<commit_message>
dynamic likes and admin changes
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -212,13 +212,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -228,6 +231,9 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -537,9 +543,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="18.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="32.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="13.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="18.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="32.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="13.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -555,17 +561,17 @@
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
+      <c r="B2" s="3"/>
       <c r="C2" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -573,10 +579,10 @@
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -584,7 +590,7 @@
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -595,7 +601,7 @@
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -606,7 +612,7 @@
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -617,7 +623,7 @@
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -628,7 +634,7 @@
       <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -639,7 +645,7 @@
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -650,7 +656,7 @@
       <c r="A11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -661,7 +667,7 @@
       <c r="A12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -672,7 +678,7 @@
       <c r="A13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -683,7 +689,7 @@
       <c r="A14" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="4" t="s">
         <v>37</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -694,7 +700,7 @@
       <c r="A15" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -705,7 +711,7 @@
       <c r="A16" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="4" t="s">
         <v>43</v>
       </c>
       <c r="C16" s="2" t="s">

</xml_diff>